<commit_message>
updated protocol and timeline
</commit_message>
<xml_diff>
--- a/Coordination/Timeline.xlsx
+++ b/Coordination/Timeline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="292" documentId="8_{281B7E56-ED8A-4BFC-B33C-8ED0E2FBF4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3839B555-96B6-42A7-A85F-9B88665E3C9B}"/>
+  <xr:revisionPtr revIDLastSave="325" documentId="8_{281B7E56-ED8A-4BFC-B33C-8ED0E2FBF4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CC4BD62-2F7B-4BCB-BC79-138AA725A6EB}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>Erstellen Sie auf diesem Arbeitsblatt einen Projektplan.
 Geben Sie den Titel dieses Projekts in Zelle B1 ein. 
@@ -304,10 +304,13 @@
     <t>Protocols</t>
   </si>
   <si>
-    <t>Thesis-Meeting 1</t>
-  </si>
-  <si>
     <t>setup project on github</t>
+  </si>
+  <si>
+    <t>Thesis-Meetings</t>
+  </si>
+  <si>
+    <t>Familiarize with the data</t>
   </si>
 </sst>
 </file>
@@ -1967,11 +1970,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BM40"/>
+  <dimension ref="A1:BM41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="6" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2745,7 +2748,7 @@
     </row>
     <row r="9" spans="1:65" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="90" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="81" t="s">
         <v>49</v>
@@ -2825,9 +2828,13 @@
       <c r="B10" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="81"/>
+      <c r="C10" s="81" t="s">
+        <v>18</v>
+      </c>
       <c r="D10" s="74"/>
-      <c r="E10" s="83"/>
+      <c r="E10" s="83">
+        <v>1.5</v>
+      </c>
       <c r="F10" s="73">
         <f>Projektanfang+6</f>
         <v>45350</v>
@@ -2910,7 +2917,7 @@
         <v>45344</v>
       </c>
       <c r="G11" s="73">
-        <f>F39</f>
+        <f>F40</f>
         <v>45478</v>
       </c>
       <c r="J11" s="21"/>
@@ -2984,7 +2991,7 @@
       <c r="G12" s="54"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11" t="str">
-        <f t="shared" ref="I12:I40" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="I12:I41" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="J12" s="21"/>
@@ -3055,23 +3062,23 @@
         <v>18</v>
       </c>
       <c r="D13" s="14">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E13" s="41">
-        <v>1.75</v>
+        <v>3</v>
       </c>
       <c r="F13" s="55">
         <f>Projektanfang</f>
         <v>45344</v>
       </c>
       <c r="G13" s="55">
-        <f>F13+12</f>
-        <v>45356</v>
+        <f>F13+19</f>
+        <v>45363</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
@@ -3141,14 +3148,16 @@
       <c r="D14" s="14">
         <v>0</v>
       </c>
-      <c r="E14" s="41"/>
+      <c r="E14" s="41">
+        <v>2.5</v>
+      </c>
       <c r="F14" s="55">
         <f>F13</f>
         <v>45344</v>
       </c>
       <c r="G14" s="55">
-        <f t="shared" ref="G14:G18" si="6">F14+12</f>
-        <v>45356</v>
+        <f>F14+19</f>
+        <v>45363</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
@@ -3220,14 +3229,16 @@
       <c r="D15" s="14">
         <v>0</v>
       </c>
-      <c r="E15" s="41"/>
+      <c r="E15" s="41">
+        <v>0.25</v>
+      </c>
       <c r="F15" s="55">
         <f>F13</f>
         <v>45344</v>
       </c>
       <c r="G15" s="55">
-        <f t="shared" si="6"/>
-        <v>45356</v>
+        <f>F15+19</f>
+        <v>45363</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -3299,23 +3310,23 @@
         <v>18</v>
       </c>
       <c r="D16" s="14">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E16" s="41">
-        <v>1.25</v>
+        <v>3.25</v>
       </c>
       <c r="F16" s="55">
         <f>F13</f>
         <v>45344</v>
       </c>
       <c r="G16" s="55">
-        <f t="shared" si="6"/>
-        <v>45356</v>
+        <f>F16+19</f>
+        <v>45363</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
@@ -3393,7 +3404,7 @@
         <v>45344</v>
       </c>
       <c r="G17" s="55">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="G17:G18" si="6">F17+12</f>
         <v>45356</v>
       </c>
       <c r="H17" s="11"/>
@@ -3458,7 +3469,7 @@
     <row r="18" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="35"/>
       <c r="B18" s="47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="41" t="s">
         <v>18</v>
@@ -3764,15 +3775,17 @@
     <row r="22" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="35"/>
       <c r="B22" s="48" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C22" s="43" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="17">
-        <v>0</v>
-      </c>
-      <c r="E22" s="43"/>
+        <v>0.1</v>
+      </c>
+      <c r="E22" s="43">
+        <v>0.25</v>
+      </c>
       <c r="F22" s="58">
         <f>F21</f>
         <v>45357</v>
@@ -3843,7 +3856,7 @@
     <row r="23" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="35"/>
       <c r="B23" s="48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="43" t="s">
         <v>18</v>
@@ -3853,12 +3866,12 @@
       </c>
       <c r="E23" s="43"/>
       <c r="F23" s="58">
-        <f>G22</f>
+        <f>F21</f>
+        <v>45357</v>
+      </c>
+      <c r="G23" s="58">
+        <f>G21</f>
         <v>45364</v>
-      </c>
-      <c r="G23" s="58">
-        <f>F34-1</f>
-        <v>45459</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
@@ -3920,9 +3933,9 @@
       <c r="BM23" s="21"/>
     </row>
     <row r="24" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="34"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="48" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="C24" s="43" t="s">
         <v>18</v>
@@ -3932,18 +3945,15 @@
       </c>
       <c r="E24" s="43"/>
       <c r="F24" s="58">
-        <f>F23</f>
+        <f>G23</f>
         <v>45364</v>
       </c>
       <c r="G24" s="58">
-        <f>G23</f>
+        <f>F35-1</f>
         <v>45459</v>
       </c>
       <c r="H24" s="11"/>
-      <c r="I24" s="11">
-        <f t="shared" si="5"/>
-        <v>96</v>
-      </c>
+      <c r="I24" s="11"/>
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
       <c r="L24" s="21"/>
@@ -3956,8 +3966,8 @@
       <c r="S24" s="21"/>
       <c r="T24" s="21"/>
       <c r="U24" s="21"/>
-      <c r="V24" s="22"/>
-      <c r="W24" s="22"/>
+      <c r="V24" s="21"/>
+      <c r="W24" s="21"/>
       <c r="X24" s="21"/>
       <c r="Y24" s="21"/>
       <c r="Z24" s="21"/>
@@ -4004,7 +4014,7 @@
     <row r="25" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="34"/>
       <c r="B25" s="48" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="C25" s="43" t="s">
         <v>18</v>
@@ -4038,8 +4048,8 @@
       <c r="S25" s="21"/>
       <c r="T25" s="21"/>
       <c r="U25" s="21"/>
-      <c r="V25" s="21"/>
-      <c r="W25" s="21"/>
+      <c r="V25" s="22"/>
+      <c r="W25" s="22"/>
       <c r="X25" s="21"/>
       <c r="Y25" s="21"/>
       <c r="Z25" s="21"/>
@@ -4085,16 +4095,29 @@
     </row>
     <row r="26" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="34"/>
-      <c r="B26" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+      <c r="B26" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="17">
+        <v>0</v>
+      </c>
+      <c r="E26" s="43"/>
+      <c r="F26" s="58">
+        <f>F25</f>
+        <v>45364</v>
+      </c>
+      <c r="G26" s="58">
+        <f>G25</f>
+        <v>45459</v>
+      </c>
       <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
+      <c r="I26" s="11">
+        <f t="shared" si="5"/>
+        <v>96</v>
+      </c>
       <c r="J26" s="21"/>
       <c r="K26" s="21"/>
       <c r="L26" s="21"/>
@@ -4154,29 +4177,16 @@
     </row>
     <row r="27" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="34"/>
-      <c r="B27" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="17">
-        <v>0</v>
-      </c>
-      <c r="E27" s="43"/>
-      <c r="F27" s="58">
-        <f>F25</f>
-        <v>45364</v>
-      </c>
-      <c r="G27" s="58">
-        <f>G25</f>
-        <v>45459</v>
-      </c>
+      <c r="B27" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
       <c r="H27" s="11"/>
-      <c r="I27" s="11">
-        <f t="shared" si="5"/>
-        <v>96</v>
-      </c>
+      <c r="I27" s="11"/>
       <c r="J27" s="21"/>
       <c r="K27" s="21"/>
       <c r="L27" s="21"/>
@@ -4193,7 +4203,7 @@
       <c r="W27" s="21"/>
       <c r="X27" s="21"/>
       <c r="Y27" s="21"/>
-      <c r="Z27" s="22"/>
+      <c r="Z27" s="21"/>
       <c r="AA27" s="21"/>
       <c r="AB27" s="21"/>
       <c r="AC27" s="21"/>
@@ -4237,7 +4247,7 @@
     <row r="28" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="34"/>
       <c r="B28" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="43" t="s">
         <v>18</v>
@@ -4247,15 +4257,18 @@
       </c>
       <c r="E28" s="43"/>
       <c r="F28" s="58">
-        <f>F27</f>
+        <f>F26</f>
         <v>45364</v>
       </c>
       <c r="G28" s="58">
-        <f>G27</f>
+        <f>G26</f>
         <v>45459</v>
       </c>
       <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
+      <c r="I28" s="11">
+        <f t="shared" si="5"/>
+        <v>96</v>
+      </c>
       <c r="J28" s="21"/>
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
@@ -4316,7 +4329,7 @@
     <row r="29" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="34"/>
       <c r="B29" s="48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="43" t="s">
         <v>18</v>
@@ -4326,11 +4339,11 @@
       </c>
       <c r="E29" s="43"/>
       <c r="F29" s="58">
-        <f t="shared" ref="F29:F33" si="7">F28</f>
+        <f>F28</f>
         <v>45364</v>
       </c>
       <c r="G29" s="58">
-        <f t="shared" ref="G29:G33" si="8">G28</f>
+        <f>G28</f>
         <v>45459</v>
       </c>
       <c r="H29" s="11"/>
@@ -4395,7 +4408,7 @@
     <row r="30" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A30" s="34"/>
       <c r="B30" s="48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="43" t="s">
         <v>18</v>
@@ -4405,11 +4418,11 @@
       </c>
       <c r="E30" s="43"/>
       <c r="F30" s="58">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="F30:F34" si="7">F29</f>
         <v>45364</v>
       </c>
       <c r="G30" s="58">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="G30:G34" si="8">G29</f>
         <v>45459</v>
       </c>
       <c r="H30" s="11"/>
@@ -4474,7 +4487,7 @@
     <row r="31" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A31" s="34"/>
       <c r="B31" s="48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="43" t="s">
         <v>18</v>
@@ -4553,7 +4566,7 @@
     <row r="32" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="34"/>
       <c r="B32" s="48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C32" s="43" t="s">
         <v>18</v>
@@ -4632,7 +4645,7 @@
     <row r="33" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="34"/>
       <c r="B33" s="48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" s="43" t="s">
         <v>18</v>
@@ -4710,23 +4723,23 @@
     </row>
     <row r="34" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="34"/>
-      <c r="B34" s="76" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="82" t="s">
+      <c r="B34" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="78">
+      <c r="D34" s="17">
         <v>0</v>
       </c>
-      <c r="E34" s="77"/>
-      <c r="F34" s="79">
-        <f>Projektanfang+116</f>
-        <v>45460</v>
-      </c>
-      <c r="G34" s="79">
-        <f>F34+4</f>
-        <v>45464</v>
+      <c r="E34" s="43"/>
+      <c r="F34" s="58">
+        <f t="shared" si="7"/>
+        <v>45364</v>
+      </c>
+      <c r="G34" s="58">
+        <f t="shared" si="8"/>
+        <v>45459</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
@@ -4746,7 +4759,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="21"/>
       <c r="Y34" s="21"/>
-      <c r="Z34" s="21"/>
+      <c r="Z34" s="22"/>
       <c r="AA34" s="21"/>
       <c r="AB34" s="21"/>
       <c r="AC34" s="21"/>
@@ -4788,22 +4801,27 @@
       <c r="BM34" s="21"/>
     </row>
     <row r="35" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="60"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="82" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="78">
+        <v>0</v>
+      </c>
+      <c r="E35" s="77"/>
+      <c r="F35" s="79">
+        <f>Projektanfang+116</f>
+        <v>45460</v>
+      </c>
+      <c r="G35" s="79">
+        <f>F35+4</f>
+        <v>45464</v>
+      </c>
       <c r="H35" s="11"/>
-      <c r="I35" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="I35" s="11"/>
       <c r="J35" s="21"/>
       <c r="K35" s="21"/>
       <c r="L35" s="21"/>
@@ -4862,31 +4880,21 @@
       <c r="BM35" s="21"/>
     </row>
     <row r="36" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A36" s="34"/>
-      <c r="B36" s="66" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="20">
-        <v>0</v>
-      </c>
-      <c r="E36" s="45">
-        <v>0</v>
-      </c>
-      <c r="F36" s="61">
-        <f>G34+1</f>
-        <v>45465</v>
-      </c>
-      <c r="G36" s="61">
-        <f>F36+13</f>
-        <v>45478</v>
-      </c>
+      <c r="A36" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="44"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="60"/>
       <c r="H36" s="11"/>
-      <c r="I36" s="11">
+      <c r="I36" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v/>
       </c>
       <c r="J36" s="21"/>
       <c r="K36" s="21"/>
@@ -4948,7 +4956,7 @@
     <row r="37" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="34"/>
       <c r="B37" s="66" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C37" s="45" t="s">
         <v>18</v>
@@ -4956,17 +4964,22 @@
       <c r="D37" s="20">
         <v>0</v>
       </c>
-      <c r="E37" s="45"/>
+      <c r="E37" s="45">
+        <v>0</v>
+      </c>
       <c r="F37" s="61">
-        <f>F36</f>
+        <f>G35+1</f>
         <v>45465</v>
       </c>
       <c r="G37" s="61">
-        <f t="shared" ref="G37:G38" si="9">F37+13</f>
+        <f>F37+13</f>
         <v>45478</v>
       </c>
       <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
+      <c r="I37" s="11">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
       <c r="J37" s="21"/>
       <c r="K37" s="21"/>
       <c r="L37" s="21"/>
@@ -5027,10 +5040,10 @@
     <row r="38" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="34"/>
       <c r="B38" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="80" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="C38" s="45" t="s">
+        <v>18</v>
       </c>
       <c r="D38" s="20">
         <v>0</v>
@@ -5041,7 +5054,7 @@
         <v>45465</v>
       </c>
       <c r="G38" s="61">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="G38:G39" si="9">F38+13</f>
         <v>45478</v>
       </c>
       <c r="H38" s="11"/>
@@ -5106,21 +5119,21 @@
     <row r="39" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="34"/>
       <c r="B39" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="45" t="s">
-        <v>18</v>
+        <v>56</v>
+      </c>
+      <c r="C39" s="80" t="s">
+        <v>57</v>
       </c>
       <c r="D39" s="20">
         <v>0</v>
       </c>
       <c r="E39" s="45"/>
       <c r="F39" s="61">
-        <f>Projektanfang+134</f>
-        <v>45478</v>
+        <f>F38</f>
+        <v>45465</v>
       </c>
       <c r="G39" s="61">
-        <f>F39</f>
+        <f t="shared" si="9"/>
         <v>45478</v>
       </c>
       <c r="H39" s="11"/>
@@ -5183,25 +5196,27 @@
       <c r="BM39" s="21"/>
     </row>
     <row r="40" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="46"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="84">
-        <f>SUM(E8:E39)</f>
-        <v>5.5</v>
-      </c>
-      <c r="F40" s="62"/>
-      <c r="G40" s="62"/>
+      <c r="A40" s="34"/>
+      <c r="B40" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="20">
+        <v>0</v>
+      </c>
+      <c r="E40" s="45"/>
+      <c r="F40" s="61">
+        <f>Projektanfang+134</f>
+        <v>45478</v>
+      </c>
+      <c r="G40" s="61">
+        <f>F40</f>
+        <v>45478</v>
+      </c>
       <c r="H40" s="11"/>
-      <c r="I40" s="11" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="I40" s="11"/>
       <c r="J40" s="21"/>
       <c r="K40" s="21"/>
       <c r="L40" s="21"/>
@@ -5259,6 +5274,83 @@
       <c r="BL40" s="21"/>
       <c r="BM40" s="21"/>
     </row>
+    <row r="41" spans="1:65" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A41" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="46"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="84">
+        <f>SUM(E8:E40)</f>
+        <v>13.25</v>
+      </c>
+      <c r="F41" s="62"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
+      <c r="T41" s="21"/>
+      <c r="U41" s="21"/>
+      <c r="V41" s="21"/>
+      <c r="W41" s="21"/>
+      <c r="X41" s="21"/>
+      <c r="Y41" s="21"/>
+      <c r="Z41" s="21"/>
+      <c r="AA41" s="21"/>
+      <c r="AB41" s="21"/>
+      <c r="AC41" s="21"/>
+      <c r="AD41" s="21"/>
+      <c r="AE41" s="21"/>
+      <c r="AF41" s="21"/>
+      <c r="AG41" s="21"/>
+      <c r="AH41" s="21"/>
+      <c r="AI41" s="21"/>
+      <c r="AJ41" s="21"/>
+      <c r="AK41" s="21"/>
+      <c r="AL41" s="21"/>
+      <c r="AM41" s="21"/>
+      <c r="AN41" s="21"/>
+      <c r="AO41" s="21"/>
+      <c r="AP41" s="21"/>
+      <c r="AQ41" s="21"/>
+      <c r="AR41" s="21"/>
+      <c r="AS41" s="21"/>
+      <c r="AT41" s="21"/>
+      <c r="AU41" s="21"/>
+      <c r="AV41" s="21"/>
+      <c r="AW41" s="21"/>
+      <c r="AX41" s="21"/>
+      <c r="AY41" s="21"/>
+      <c r="AZ41" s="21"/>
+      <c r="BA41" s="21"/>
+      <c r="BB41" s="21"/>
+      <c r="BC41" s="21"/>
+      <c r="BD41" s="21"/>
+      <c r="BE41" s="21"/>
+      <c r="BF41" s="21"/>
+      <c r="BG41" s="21"/>
+      <c r="BH41" s="21"/>
+      <c r="BI41" s="21"/>
+      <c r="BJ41" s="21"/>
+      <c r="BK41" s="21"/>
+      <c r="BL41" s="21"/>
+      <c r="BM41" s="21"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="C3:D3"/>
@@ -5273,7 +5365,7 @@
     <mergeCell ref="X4:AD4"/>
     <mergeCell ref="AE4:AK4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:E7 D27:D40 D8:D25">
+  <conditionalFormatting sqref="D7:E7 D28:D41 D8:D26">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5287,12 +5379,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5:BM40">
+  <conditionalFormatting sqref="J5:BM41">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:BM40">
+  <conditionalFormatting sqref="J7:BM41">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=J$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=J$5)</formula>
     </cfRule>
@@ -5327,7 +5419,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:E7 D27:D40 D8:D25</xm:sqref>
+          <xm:sqref>D7:E7 D28:D41 D8:D26</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
updated timeline and protocol notes
</commit_message>
<xml_diff>
--- a/Coordination/Timeline.xlsx
+++ b/Coordination/Timeline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="410" documentId="8_{281B7E56-ED8A-4BFC-B33C-8ED0E2FBF4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{247BB2F6-C68E-4364-8C5E-BA88823D29FD}"/>
+  <xr:revisionPtr revIDLastSave="431" documentId="8_{281B7E56-ED8A-4BFC-B33C-8ED0E2FBF4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E94A7A67-9898-4355-A5D1-7D3C3B788608}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1973,8 +1973,8 @@
   <dimension ref="A1:FG41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4657,10 +4657,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="14">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E14" s="41">
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="F14" s="55">
         <f>F13</f>
@@ -5017,10 +5017,10 @@
         <v>18</v>
       </c>
       <c r="D16" s="14">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E16" s="41">
-        <v>7</v>
+        <v>7.5</v>
       </c>
       <c r="F16" s="55">
         <f>F13</f>
@@ -5899,7 +5899,7 @@
         <v>0.8</v>
       </c>
       <c r="E21" s="43">
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="F21" s="58">
         <v>45366</v>
@@ -6256,10 +6256,10 @@
         <v>18</v>
       </c>
       <c r="D23" s="17">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E23" s="43">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F23" s="58">
         <f>F21</f>
@@ -7506,8 +7506,8 @@
         <v>45438</v>
       </c>
       <c r="G30" s="58">
-        <f t="shared" ref="G30:G34" si="119">G29</f>
-        <v>45459</v>
+        <f>F29</f>
+        <v>45453</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
@@ -7679,12 +7679,12 @@
       </c>
       <c r="E31" s="43"/>
       <c r="F31" s="58">
-        <f t="shared" ref="F31:F34" si="120">F30</f>
+        <f t="shared" ref="F31:F33" si="119">F30</f>
         <v>45438</v>
       </c>
       <c r="G31" s="58">
-        <f t="shared" si="119"/>
-        <v>45459</v>
+        <f t="shared" ref="G31:G33" si="120">G30</f>
+        <v>45453</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
@@ -7856,12 +7856,12 @@
       </c>
       <c r="E32" s="43"/>
       <c r="F32" s="58">
-        <f t="shared" si="120"/>
+        <f>F31</f>
         <v>45438</v>
       </c>
       <c r="G32" s="58">
-        <f t="shared" si="119"/>
-        <v>45459</v>
+        <f>G31</f>
+        <v>45453</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
@@ -8033,12 +8033,12 @@
       </c>
       <c r="E33" s="43"/>
       <c r="F33" s="58">
+        <f t="shared" si="119"/>
+        <v>45438</v>
+      </c>
+      <c r="G33" s="58">
         <f t="shared" si="120"/>
-        <v>45438</v>
-      </c>
-      <c r="G33" s="58">
-        <f t="shared" si="119"/>
-        <v>45459</v>
+        <v>45453</v>
       </c>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
@@ -8210,11 +8210,11 @@
       </c>
       <c r="E34" s="43"/>
       <c r="F34" s="58">
-        <f t="shared" si="120"/>
-        <v>45438</v>
+        <f>F29</f>
+        <v>45453</v>
       </c>
       <c r="G34" s="58">
-        <f t="shared" si="119"/>
+        <f>G29</f>
         <v>45459</v>
       </c>
       <c r="H34" s="11"/>
@@ -9447,7 +9447,7 @@
       <c r="D41" s="10"/>
       <c r="E41" s="84">
         <f>SUM(E8:E40)</f>
-        <v>34.75</v>
+        <v>42.5</v>
       </c>
       <c r="F41" s="62"/>
       <c r="G41" s="62"/>
@@ -9805,35 +9805,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10121,27 +10092,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708DBB9E-6D89-4A94-9DC5-964B7833E11C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10160,4 +10140,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated protocols and timeline
</commit_message>
<xml_diff>
--- a/Coordination/Timeline.xlsx
+++ b/Coordination/Timeline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="445" documentId="8_{281B7E56-ED8A-4BFC-B33C-8ED0E2FBF4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99A497A7-5E12-4BD9-A331-8780DF1034AF}"/>
+  <xr:revisionPtr revIDLastSave="450" documentId="8_{281B7E56-ED8A-4BFC-B33C-8ED0E2FBF4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F7A0755-4465-43A4-9FAA-005124071A6B}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1704,10 +1704,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1977,8 +1973,8 @@
   <dimension ref="A1:FG41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3782,7 +3778,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="83">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="F9" s="73">
         <f>Projektanfang</f>
@@ -4131,7 +4127,7 @@
         <v>0.05</v>
       </c>
       <c r="E11" s="83">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F11" s="73">
         <f>Projektanfang</f>
@@ -6263,7 +6259,7 @@
         <v>0.8</v>
       </c>
       <c r="E23" s="43">
-        <v>17.5</v>
+        <v>23.5</v>
       </c>
       <c r="F23" s="58">
         <f>F21</f>
@@ -7148,7 +7144,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="43">
-        <v>2.75</v>
+        <v>4.25</v>
       </c>
       <c r="F28" s="58">
         <f>F24</f>
@@ -9453,7 +9449,7 @@
       <c r="D41" s="10"/>
       <c r="E41" s="84">
         <f>SUM(E8:E40)</f>
-        <v>53.5</v>
+        <v>62.25</v>
       </c>
       <c r="F41" s="62"/>
       <c r="G41" s="62"/>
@@ -9619,6 +9615,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="DY4:EE4"/>
+    <mergeCell ref="EF4:EL4"/>
+    <mergeCell ref="EM4:ES4"/>
+    <mergeCell ref="ET4:EZ4"/>
+    <mergeCell ref="FA4:FG4"/>
+    <mergeCell ref="CP4:CV4"/>
+    <mergeCell ref="CW4:DC4"/>
+    <mergeCell ref="DD4:DJ4"/>
+    <mergeCell ref="DK4:DQ4"/>
+    <mergeCell ref="DR4:DX4"/>
     <mergeCell ref="BN4:BT4"/>
     <mergeCell ref="BU4:CA4"/>
     <mergeCell ref="CB4:CH4"/>
@@ -9634,16 +9640,6 @@
     <mergeCell ref="Q4:W4"/>
     <mergeCell ref="X4:AD4"/>
     <mergeCell ref="AE4:AK4"/>
-    <mergeCell ref="CP4:CV4"/>
-    <mergeCell ref="CW4:DC4"/>
-    <mergeCell ref="DD4:DJ4"/>
-    <mergeCell ref="DK4:DQ4"/>
-    <mergeCell ref="DR4:DX4"/>
-    <mergeCell ref="DY4:EE4"/>
-    <mergeCell ref="EF4:EL4"/>
-    <mergeCell ref="EM4:ES4"/>
-    <mergeCell ref="ET4:EZ4"/>
-    <mergeCell ref="FA4:FG4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E7 D28:D41 D8:D26">
     <cfRule type="dataBar" priority="14">
@@ -10099,6 +10095,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -10116,15 +10121,6 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10149,6 +10145,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -10158,12 +10162,4 @@
     <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated timeline and protocol, added fluxnet data
</commit_message>
<xml_diff>
--- a/Coordination/Timeline.xlsx
+++ b/Coordination/Timeline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="450" documentId="8_{281B7E56-ED8A-4BFC-B33C-8ED0E2FBF4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F7A0755-4465-43A4-9FAA-005124071A6B}"/>
+  <xr:revisionPtr revIDLastSave="451" documentId="8_{281B7E56-ED8A-4BFC-B33C-8ED0E2FBF4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F66907FD-12BF-448E-808B-A8A084E6EFBF}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1973,8 +1973,8 @@
   <dimension ref="A1:FG41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="6" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6259,7 +6259,7 @@
         <v>0.8</v>
       </c>
       <c r="E23" s="43">
-        <v>23.5</v>
+        <v>27.5</v>
       </c>
       <c r="F23" s="58">
         <f>F21</f>
@@ -9449,7 +9449,7 @@
       <c r="D41" s="10"/>
       <c r="E41" s="84">
         <f>SUM(E8:E40)</f>
-        <v>62.25</v>
+        <v>66.25</v>
       </c>
       <c r="F41" s="62"/>
       <c r="G41" s="62"/>
@@ -9615,16 +9615,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="DY4:EE4"/>
-    <mergeCell ref="EF4:EL4"/>
-    <mergeCell ref="EM4:ES4"/>
-    <mergeCell ref="ET4:EZ4"/>
-    <mergeCell ref="FA4:FG4"/>
-    <mergeCell ref="CP4:CV4"/>
-    <mergeCell ref="CW4:DC4"/>
-    <mergeCell ref="DD4:DJ4"/>
-    <mergeCell ref="DK4:DQ4"/>
-    <mergeCell ref="DR4:DX4"/>
     <mergeCell ref="BN4:BT4"/>
     <mergeCell ref="BU4:CA4"/>
     <mergeCell ref="CB4:CH4"/>
@@ -9640,6 +9630,16 @@
     <mergeCell ref="Q4:W4"/>
     <mergeCell ref="X4:AD4"/>
     <mergeCell ref="AE4:AK4"/>
+    <mergeCell ref="CP4:CV4"/>
+    <mergeCell ref="CW4:DC4"/>
+    <mergeCell ref="DD4:DJ4"/>
+    <mergeCell ref="DK4:DQ4"/>
+    <mergeCell ref="DR4:DX4"/>
+    <mergeCell ref="DY4:EE4"/>
+    <mergeCell ref="EF4:EL4"/>
+    <mergeCell ref="EM4:ES4"/>
+    <mergeCell ref="ET4:EZ4"/>
+    <mergeCell ref="FA4:FG4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E7 D28:D41 D8:D26">
     <cfRule type="dataBar" priority="14">
@@ -9807,6 +9807,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10094,36 +10123,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708DBB9E-6D89-4A94-9DC5-964B7833E11C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10142,24 +10162,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated timeline and protocol
</commit_message>
<xml_diff>
--- a/Coordination/Timeline.xlsx
+++ b/Coordination/Timeline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="461" documentId="8_{281B7E56-ED8A-4BFC-B33C-8ED0E2FBF4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF1E3690-A3DC-45AB-972C-9ABD27FA72F8}"/>
+  <xr:revisionPtr revIDLastSave="495" documentId="8_{281B7E56-ED8A-4BFC-B33C-8ED0E2FBF4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86C33D5E-1669-4733-B47D-4811D0F084B6}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1973,8 +1973,8 @@
   <dimension ref="A1:FG41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <pane ySplit="6" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -3952,7 +3952,7 @@
       </c>
       <c r="D10" s="74"/>
       <c r="E10" s="83">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="F10" s="73">
         <f>Projektanfang+6</f>
@@ -4127,7 +4127,7 @@
         <v>0.05</v>
       </c>
       <c r="E11" s="83">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="F11" s="73">
         <f>Projektanfang</f>
@@ -6256,7 +6256,7 @@
         <v>18</v>
       </c>
       <c r="D23" s="17">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E23" s="43">
         <v>37</v>
@@ -6443,8 +6443,8 @@
         <v>45404</v>
       </c>
       <c r="G24" s="58">
-        <f>F24+21</f>
-        <v>45425</v>
+        <f>F24+35</f>
+        <v>45439</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
@@ -6619,11 +6619,11 @@
       </c>
       <c r="F25" s="58">
         <f>G24</f>
-        <v>45425</v>
+        <v>45439</v>
       </c>
       <c r="G25" s="58">
         <f>F25+14</f>
-        <v>45439</v>
+        <v>45453</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11">
@@ -6798,7 +6798,7 @@
       </c>
       <c r="E26" s="43"/>
       <c r="F26" s="58">
-        <f>G25</f>
+        <f>F25</f>
         <v>45439</v>
       </c>
       <c r="G26" s="58">
@@ -7144,7 +7144,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="43">
-        <v>5.5</v>
+        <v>8.25</v>
       </c>
       <c r="F28" s="58">
         <f>F24</f>
@@ -7152,12 +7152,12 @@
       </c>
       <c r="G28" s="58">
         <f>F35-1</f>
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="11">
         <f t="shared" si="117"/>
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="J28" s="21"/>
       <c r="K28" s="21"/>
@@ -7328,11 +7328,11 @@
       <c r="E29" s="43"/>
       <c r="F29" s="58">
         <f>F35-7</f>
-        <v>45453</v>
+        <v>45460</v>
       </c>
       <c r="G29" s="58">
         <f>G28</f>
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
@@ -7502,14 +7502,15 @@
       <c r="D30" s="17">
         <v>0</v>
       </c>
-      <c r="E30" s="43"/>
+      <c r="E30" s="43">
+        <v>3.75</v>
+      </c>
       <c r="F30" s="58">
-        <f>G26</f>
-        <v>45453</v>
+        <v>45425</v>
       </c>
       <c r="G30" s="58">
-        <f>F29</f>
-        <v>45453</v>
+        <f>F30+7</f>
+        <v>45432</v>
       </c>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
@@ -7679,14 +7680,16 @@
       <c r="D31" s="17">
         <v>0</v>
       </c>
-      <c r="E31" s="43"/>
+      <c r="E31" s="43">
+        <v>2</v>
+      </c>
       <c r="F31" s="58">
         <f t="shared" ref="F31:F33" si="119">F30</f>
-        <v>45453</v>
+        <v>45425</v>
       </c>
       <c r="G31" s="58">
-        <f t="shared" ref="G31:G33" si="120">G30</f>
-        <v>45453</v>
+        <f t="shared" ref="G31" si="120">G30</f>
+        <v>45432</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
@@ -7858,12 +7861,12 @@
       </c>
       <c r="E32" s="43"/>
       <c r="F32" s="58">
-        <f>F31</f>
-        <v>45453</v>
+        <f>F29</f>
+        <v>45460</v>
       </c>
       <c r="G32" s="58">
-        <f>G31</f>
-        <v>45453</v>
+        <f>G29</f>
+        <v>45466</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
@@ -8036,11 +8039,11 @@
       <c r="E33" s="43"/>
       <c r="F33" s="58">
         <f t="shared" si="119"/>
-        <v>45453</v>
+        <v>45460</v>
       </c>
       <c r="G33" s="58">
-        <f t="shared" si="120"/>
-        <v>45453</v>
+        <f>G32</f>
+        <v>45466</v>
       </c>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
@@ -8213,11 +8216,11 @@
       <c r="E34" s="43"/>
       <c r="F34" s="58">
         <f>F29</f>
-        <v>45453</v>
+        <v>45460</v>
       </c>
       <c r="G34" s="58">
         <f>G29</f>
-        <v>45459</v>
+        <v>45466</v>
       </c>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
@@ -8389,12 +8392,12 @@
       </c>
       <c r="E35" s="77"/>
       <c r="F35" s="79">
-        <f>Projektanfang+116</f>
-        <v>45460</v>
+        <f>Projektanfang+123</f>
+        <v>45467</v>
       </c>
       <c r="G35" s="79">
         <f>F35+4</f>
-        <v>45464</v>
+        <v>45471</v>
       </c>
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
@@ -8740,17 +8743,17 @@
         <v>0</v>
       </c>
       <c r="F37" s="61">
-        <f>G35+1</f>
-        <v>45465</v>
+        <f>F35+1</f>
+        <v>45468</v>
       </c>
       <c r="G37" s="61">
-        <f>F37+13</f>
+        <f>F37+10</f>
         <v>45478</v>
       </c>
       <c r="H37" s="11"/>
       <c r="I37" s="11">
         <f t="shared" si="117"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J37" s="21"/>
       <c r="K37" s="21"/>
@@ -8920,11 +8923,11 @@
       </c>
       <c r="E38" s="45"/>
       <c r="F38" s="61">
-        <f>F37</f>
-        <v>45465</v>
+        <f>F37+6</f>
+        <v>45474</v>
       </c>
       <c r="G38" s="61">
-        <f t="shared" ref="G38:G39" si="121">F38+13</f>
+        <f>F38+4</f>
         <v>45478</v>
       </c>
       <c r="H38" s="11"/>
@@ -9097,12 +9100,12 @@
       </c>
       <c r="E39" s="45"/>
       <c r="F39" s="61">
-        <f>F38</f>
-        <v>45465</v>
+        <f>F35</f>
+        <v>45467</v>
       </c>
       <c r="G39" s="61">
-        <f t="shared" si="121"/>
-        <v>45478</v>
+        <f>F39+6</f>
+        <v>45473</v>
       </c>
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
@@ -9449,7 +9452,7 @@
       <c r="D41" s="10"/>
       <c r="E41" s="84">
         <f>SUM(E8:E40)</f>
-        <v>82</v>
+        <v>91.75</v>
       </c>
       <c r="F41" s="62"/>
       <c r="G41" s="62"/>
@@ -9615,6 +9618,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="DY4:EE4"/>
+    <mergeCell ref="EF4:EL4"/>
+    <mergeCell ref="EM4:ES4"/>
+    <mergeCell ref="ET4:EZ4"/>
+    <mergeCell ref="FA4:FG4"/>
+    <mergeCell ref="CP4:CV4"/>
+    <mergeCell ref="CW4:DC4"/>
+    <mergeCell ref="DD4:DJ4"/>
+    <mergeCell ref="DK4:DQ4"/>
+    <mergeCell ref="DR4:DX4"/>
     <mergeCell ref="BN4:BT4"/>
     <mergeCell ref="BU4:CA4"/>
     <mergeCell ref="CB4:CH4"/>
@@ -9630,16 +9643,6 @@
     <mergeCell ref="Q4:W4"/>
     <mergeCell ref="X4:AD4"/>
     <mergeCell ref="AE4:AK4"/>
-    <mergeCell ref="CP4:CV4"/>
-    <mergeCell ref="CW4:DC4"/>
-    <mergeCell ref="DD4:DJ4"/>
-    <mergeCell ref="DK4:DQ4"/>
-    <mergeCell ref="DR4:DX4"/>
-    <mergeCell ref="DY4:EE4"/>
-    <mergeCell ref="EF4:EL4"/>
-    <mergeCell ref="EM4:ES4"/>
-    <mergeCell ref="ET4:EZ4"/>
-    <mergeCell ref="FA4:FG4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E7 D28:D41 D8:D26">
     <cfRule type="dataBar" priority="14">
@@ -9807,35 +9810,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10123,27 +10097,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708DBB9E-6D89-4A94-9DC5-964B7833E11C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10162,4 +10145,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>